<commit_message>
Patch for In argument + Test fixes
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
@@ -15,30 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
     <x:t>File Number</x:t>
-  </x:si>
-  <x:si>
-    <x:t>File Number - Confidence</x:t>
   </x:si>
   <x:si>
     <x:t>Dated</x:t>
   </x:si>
   <x:si>
-    <x:t>Dated - Confidence</x:t>
-  </x:si>
-  <x:si>
     <x:t>Effective</x:t>
   </x:si>
   <x:si>
-    <x:t>Effective - Confidence</x:t>
-  </x:si>
-  <x:si>
     <x:t>801193487</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
   </x:si>
   <x:si>
     <x:t>11/12/2009</x:t>
@@ -392,13 +380,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F2"/>
+  <x:dimension ref="A1:C2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -408,34 +396,16 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:6">
-      <x:c r="A2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -452,13 +422,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F2"/>
+  <x:dimension ref="A1:C2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -468,34 +438,16 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:6">
-      <x:c r="A2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Autocorrect OCR mistakes - updated annotations, caches and user guide
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <x:si>
     <x:t>File Number</x:t>
   </x:si>
@@ -26,10 +26,16 @@
     <x:t>Effective</x:t>
   </x:si>
   <x:si>
+    <x:t>State</x:t>
+  </x:si>
+  <x:si>
     <x:t>801193487</x:t>
   </x:si>
   <x:si>
     <x:t>11/12/2009</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STATE OF MndstcT TEXAS THL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -380,13 +386,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -396,16 +402,22 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -422,13 +434,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -438,16 +450,22 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Manual merge of AutocorrectOcrMistakes feature into CrossPlatform_Template; Affected files (pt0) - config, userguide, taxonomy, tests & mocks folders, main attended, main action center, extract, extract validation.
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <x:si>
     <x:t>File Number</x:t>
   </x:si>
@@ -26,10 +26,16 @@
     <x:t>Effective</x:t>
   </x:si>
   <x:si>
+    <x:t>State</x:t>
+  </x:si>
+  <x:si>
     <x:t>801193487</x:t>
   </x:si>
   <x:si>
     <x:t>11/12/2009</x:t>
+  </x:si>
+  <x:si>
+    <x:t>STATE OF MndstcT TEXAS THL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -380,13 +386,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -396,16 +402,22 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -422,13 +434,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -438,16 +450,22 @@
       <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Update packages for Document Understanding template.
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <x:si>
     <x:t>File Number</x:t>
   </x:si>
@@ -33,9 +33,6 @@
   </x:si>
   <x:si>
     <x:t>11/12/2009</x:t>
-  </x:si>
-  <x:si>
-    <x:t>STATE OF S TEXAS 3H1</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -416,9 +413,6 @@
       <x:c r="C2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -464,9 +458,6 @@
       <x:c r="C2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Update digitize,classify and extract RPA test data.Change UiPath Test package.Update release version.
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/ExportMergedDocuments_1-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <x:si>
     <x:t>File Number</x:t>
   </x:si>
@@ -29,13 +29,10 @@
     <x:t>State</x:t>
   </x:si>
   <x:si>
-    <x:t>801193487</x:t>
-  </x:si>
-  <x:si>
     <x:t>11/12/2009</x:t>
   </x:si>
   <x:si>
-    <x:t>STATE OF S TEXAS 3H1</x:t>
+    <x:t>STATE OF EXAS 3HL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -407,17 +404,14 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -455,17 +449,14 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>